<commit_message>
Fix resilié cloture issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2023.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2023.xlsx
@@ -471,7 +471,7 @@
         <v>--</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="3">
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>139150</v>
+        <v>154150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix XML mtn issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2023.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_9_2023.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,19 +429,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v xml:space="preserve">952/CASA ANFA </v>
+        <v>389/AOURIR/AV1</v>
       </c>
       <c r="B2" t="str">
         <v>Point de vente</v>
       </c>
       <c r="C2" t="str">
-        <v>K254546</v>
+        <v>FF</v>
       </c>
       <c r="D2" t="str">
-        <v>MANAL JAJA</v>
+        <v>AGENCE KHATABI</v>
       </c>
       <c r="E2" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F2" t="str">
         <v>mensuelle</v>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>15000</v>
+        <v>3000</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -471,21 +471,21 @@
         <v>--</v>
       </c>
       <c r="O2">
-        <v>15000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>222/RABAT /AV1</v>
+        <v>389/AOURIR/AV1</v>
       </c>
       <c r="B3" t="str">
-        <v>Direction régionale</v>
+        <v>Point de vente</v>
       </c>
       <c r="C3" t="str">
-        <v>K2574857</v>
+        <v>A6743213</v>
       </c>
       <c r="D3" t="str">
-        <v>NADIA JJEE</v>
+        <v>ZEROUALI IBTISSAM</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -494,16 +494,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H3">
-        <v>13333.33</v>
+        <v>4500</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>2000</v>
+        <v>450</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -518,24 +518,24 @@
         <v>--</v>
       </c>
       <c r="O3">
-        <v>11333.33</v>
+        <v>4050</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>222/RABAT /AV1</v>
+        <v>001/SUP SUD</v>
       </c>
       <c r="B4" t="str">
-        <v>Direction régionale</v>
+        <v>Supervision</v>
       </c>
       <c r="C4" t="str">
-        <v>F4767464</v>
+        <v>1098777</v>
       </c>
       <c r="D4" t="str">
-        <v xml:space="preserve">MED FARID </v>
+        <v>AGENCE LAHLOU</v>
       </c>
       <c r="E4" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F4" t="str">
         <v>mensuelle</v>
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1666.67</v>
+        <v>3000</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -565,21 +565,21 @@
         <v>--</v>
       </c>
       <c r="O4">
-        <v>1666.67</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>222/RABAT /AV1</v>
+        <v>001/SUP SUD</v>
       </c>
       <c r="B5" t="str">
-        <v>Direction régionale</v>
+        <v>Supervision</v>
       </c>
       <c r="C5" t="str">
-        <v>M564634</v>
+        <v/>
       </c>
       <c r="D5" t="str">
-        <v>LATIFA FIFA</v>
+        <v>BENNIS MOHAMED</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -591,13 +591,13 @@
         <v>10</v>
       </c>
       <c r="H5">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -612,21 +612,21 @@
         <v>--</v>
       </c>
       <c r="O5">
-        <v>4500</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>966/RABAT SUP1/AV1</v>
+        <v>001/SUP SUD</v>
       </c>
       <c r="B6" t="str">
         <v>Supervision</v>
       </c>
       <c r="C6" t="str">
-        <v>L5453746</v>
+        <v>B12346</v>
       </c>
       <c r="D6" t="str">
-        <v>MERYEM RARA</v>
+        <v>BAKKALI MOHAMED</v>
       </c>
       <c r="E6" t="str">
         <v>non</v>
@@ -664,16 +664,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>966/RABAT SUP1/AV1</v>
+        <v>988/DIRECTION CAPITAL SOFT</v>
       </c>
       <c r="B7" t="str">
-        <v>Supervision</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C7" t="str">
-        <v>KL254545</v>
+        <v>B12346</v>
       </c>
       <c r="D7" t="str">
-        <v>LAILA JJJJ</v>
+        <v>BAKKALI MOHAMED</v>
       </c>
       <c r="E7" t="str">
         <v>non</v>
@@ -682,16 +682,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>4500</v>
+        <v>2000</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -706,39 +706,39 @@
         <v>--</v>
       </c>
       <c r="O7">
-        <v>4050</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>966/RABAT SUP1/AV1</v>
+        <v>988/DIRECTION CAPITAL SOFT</v>
       </c>
       <c r="B8" t="str">
-        <v>Supervision</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C8" t="str">
-        <v>354643</v>
+        <v>A123456</v>
       </c>
       <c r="D8" t="str">
-        <v>STE LOC 10</v>
+        <v>YOUSSEF</v>
       </c>
       <c r="E8" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F8" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H8">
-        <v>7500</v>
+        <v>4000</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -753,21 +753,21 @@
         <v>--</v>
       </c>
       <c r="O8">
-        <v>7500</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>800/PV FES 1</v>
+        <v>988/DIRECTION CAPITAL SOFT</v>
       </c>
       <c r="B9" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C9" t="str">
-        <v>L3563563</v>
+        <v>J207703</v>
       </c>
       <c r="D9" t="str">
-        <v xml:space="preserve">ALAAL JAJA </v>
+        <v>ACHENGLI LAILA</v>
       </c>
       <c r="E9" t="str">
         <v>non</v>
@@ -776,16 +776,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -800,39 +800,39 @@
         <v>--</v>
       </c>
       <c r="O9">
-        <v>5400</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>558/CASA LOISIS</v>
+        <v>604/ERRAHMA</v>
       </c>
       <c r="B10" t="str">
         <v>Point de vente</v>
       </c>
       <c r="C10" t="str">
-        <v>J5454525</v>
+        <v>19087</v>
       </c>
       <c r="D10" t="str">
-        <v>LALA NANA</v>
+        <v>AGENCE ESSALAM</v>
       </c>
       <c r="E10" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F10" t="str">
-        <v>annuelle</v>
+        <v>mensuelle</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>120000</v>
+        <v>3333.33</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>18000</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -847,59 +847,153 @@
         <v>--</v>
       </c>
       <c r="O10">
-        <v>102000</v>
+        <v>3333.33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
+        <v>604/ERRAHMA</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C11" t="str">
+        <v>A6743213</v>
+      </c>
+      <c r="D11" t="str">
+        <v>ZEROUALI IBTISSAM</v>
+      </c>
+      <c r="E11" t="str">
+        <v>non</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>3333.33</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>333.33</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="str">
+        <v>--</v>
+      </c>
+      <c r="O11">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>604/ERRAHMA</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <v>EL OUAZZANI SIHAM</v>
+      </c>
+      <c r="E12" t="str">
+        <v>non</v>
+      </c>
+      <c r="F12" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>3333.33</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>333.33</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="str">
+        <v>--</v>
+      </c>
+      <c r="O12">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B11" t="str">
+      <c r="B13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C11" t="str">
+      <c r="C13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D11" t="str">
+      <c r="D13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E11" t="str">
+      <c r="E13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F11" t="str">
+      <c r="F13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G11" t="str">
+      <c r="G13" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H11">
-        <v>176000</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>21850</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>154150</v>
+      <c r="H13">
+        <v>34499.99</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>2116.66</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>32383.33</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>